<commit_message>
Noticed a mistake with Angelic Egg. Also, finished its art and put together its card and a collage of all typal searchers, both the ones Konami has printed and my custom cards.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Searchers/Designs/Typal Searchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AF488E-99BF-41BA-918E-5F1EF64D4EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CED1FE-9B66-4CD7-BB92-0E50A76B58F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -607,21 +607,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,7 +1002,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,24 +1249,28 @@
       <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="7">
         <v>3</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="7">
+        <v>1100</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1200</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="7" t="s">
         <v>71</v>
       </c>
       <c r="N7" t="s">
@@ -1536,28 +1535,28 @@
       <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>4</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <v>1000</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>1300</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1696,7 +1695,7 @@
       <c r="K19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="4" t="s">
         <v>84</v>
       </c>
       <c r="N19" t="s">
@@ -1918,7 +1917,7 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="7" t="s">
+      <c r="E27" t="s">
         <v>57</v>
       </c>
       <c r="F27">
@@ -1927,7 +1926,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E28" s="7" t="s">
+      <c r="E28" t="s">
         <v>59</v>
       </c>
       <c r="F28">
@@ -1938,7 +1937,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="7" t="s">
+      <c r="E29" t="s">
         <v>58</v>
       </c>
       <c r="F29">
@@ -1947,7 +1946,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E30" s="7" t="s">
+      <c r="E30" t="s">
         <v>105</v>
       </c>
       <c r="F30">
@@ -2002,7 +2001,7 @@
     <col min="9" max="9" width="68.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2028,7 +2027,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2041,24 +2040,21 @@
       <c r="D2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="5" t="s">
         <v>114</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2071,24 +2067,20 @@
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G3" s="7"/>
       <c r="H3" s="5" t="s">
         <v>109</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2101,24 +2093,21 @@
       <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" t="s">
         <v>125</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="5" t="s">
         <v>116</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2131,24 +2120,21 @@
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="5" t="s">
         <v>156</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2161,24 +2147,21 @@
       <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" t="s">
         <v>168</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2191,22 +2174,18 @@
       <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2219,24 +2198,20 @@
       <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" t="s">
         <v>134</v>
       </c>
-      <c r="G8" s="7"/>
       <c r="H8" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2249,24 +2224,20 @@
       <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="7"/>
       <c r="H9" s="5" t="s">
         <v>113</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2279,24 +2250,20 @@
       <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="7"/>
       <c r="H10" s="5" t="s">
         <v>163</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2309,22 +2276,17 @@
       <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2337,24 +2299,20 @@
       <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" t="s">
         <v>169</v>
       </c>
-      <c r="G12" s="7"/>
       <c r="H12" s="5" t="s">
         <v>110</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2367,22 +2325,17 @@
       <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="7"/>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2395,22 +2348,17 @@
       <c r="D14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7" t="s">
+      <c r="F14" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2423,24 +2371,20 @@
       <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G15" s="7"/>
       <c r="H15" s="5" t="s">
         <v>117</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2453,22 +2397,19 @@
       <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" t="s">
         <v>135</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="12" t="s">
+      <c r="G16" s="1"/>
+      <c r="H16" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -2483,22 +2424,18 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="7"/>
       <c r="H17" s="5" t="s">
         <v>119</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -2513,22 +2450,18 @@
       <c r="D18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" t="s">
         <v>128</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G18" s="7"/>
       <c r="H18" s="5" t="s">
         <v>108</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -2543,22 +2476,19 @@
       <c r="D19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" t="s">
         <v>124</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="5" t="s">
         <v>115</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="11"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2573,22 +2503,18 @@
       <c r="D20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="7"/>
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -2603,22 +2529,19 @@
       <c r="D21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="7"/>
       <c r="H21" s="5" t="s">
         <v>111</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="10"/>
+      <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2633,16 +2556,9 @@
       <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -2657,16 +2573,12 @@
       <c r="D23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2681,16 +2593,9 @@
       <c r="D24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -2705,19 +2610,12 @@
       <c r="D25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4 E12 E20 H1:I1 H3 H7:I7 H22:H25 H18:I21 H12:I15 H16:H17 I16 H8:H11">
+  <conditionalFormatting sqref="H1:I1 H3 E4 H7:I7 H8:H11 E12 H12:I15 I16 H16:H17 H18:I21 E20 H22:H25">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"DARK"</formula>
     </cfRule>

</xml_diff>